<commit_message>
[FIX] ssu ribosomal; Final tree [WILDCARD] The Black Death.
</commit_message>
<xml_diff>
--- a/organisms_rna/report.xlsx
+++ b/organisms_rna/report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/Papers/bit analysis/bit-analysis/organisms_rna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="14_{0DE95665-A383-4FB8-AE6D-221C9E1F430A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{13B7A54A-00F3-41BC-B4EE-4AA479E8A577}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="14_{0DE95665-A383-4FB8-AE6D-221C9E1F430A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{36A6D34D-4D81-4672-8223-45BC89B5C579}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="342">
   <si>
     <t>name</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>9606</t>
-  </si>
-  <si>
-    <t>2334371</t>
   </si>
   <si>
     <t>GCF_000001405.39</t>
@@ -1414,7 +1411,7 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1518,23 +1515,23 @@
       <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>2334371</v>
+      </c>
+      <c r="G3" t="s">
         <v>26</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>29</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>31</v>
       </c>
       <c r="L3" t="b">
         <v>1</v>
@@ -1542,37 +1539,37 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>34</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
         <v>35</v>
       </c>
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>36</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>37</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>38</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>39</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>40</v>
-      </c>
-      <c r="K4" t="s">
-        <v>41</v>
       </c>
       <c r="L4" t="b">
         <v>1</v>
@@ -1580,37 +1577,37 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
         <v>42</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>43</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>44</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
         <v>45</v>
       </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>46</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>47</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>48</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>49</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>50</v>
-      </c>
-      <c r="K5" t="s">
-        <v>51</v>
       </c>
       <c r="L5" t="b">
         <v>1</v>
@@ -1618,37 +1615,37 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
         <v>52</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
         <v>53</v>
       </c>
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
         <v>54</v>
       </c>
-      <c r="E6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>55</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>56</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>57</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>58</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>59</v>
-      </c>
-      <c r="K6" t="s">
-        <v>60</v>
       </c>
       <c r="L6" t="b">
         <v>1</v>
@@ -1656,37 +1653,37 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
         <v>61</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>62</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>63</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" t="s">
         <v>64</v>
       </c>
-      <c r="E7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>65</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>66</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>67</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>68</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>69</v>
-      </c>
-      <c r="K7" t="s">
-        <v>70</v>
       </c>
       <c r="L7" t="b">
         <v>1</v>
@@ -1694,37 +1691,37 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
         <v>71</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>72</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>73</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" t="s">
         <v>74</v>
       </c>
-      <c r="E8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>75</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>76</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>77</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>78</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>79</v>
-      </c>
-      <c r="K8" t="s">
-        <v>80</v>
       </c>
       <c r="L8" t="b">
         <v>1</v>
@@ -1732,37 +1729,37 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
         <v>81</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>82</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>83</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" t="s">
         <v>84</v>
       </c>
-      <c r="E9" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>85</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>86</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>87</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>88</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>89</v>
-      </c>
-      <c r="K9" t="s">
-        <v>90</v>
       </c>
       <c r="L9" t="b">
         <v>1</v>
@@ -1770,37 +1767,37 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" t="s">
         <v>91</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>92</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>93</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" t="s">
         <v>94</v>
       </c>
-      <c r="E10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>95</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>96</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>97</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>98</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>99</v>
-      </c>
-      <c r="K10" t="s">
-        <v>100</v>
       </c>
       <c r="L10" t="b">
         <v>1</v>
@@ -1808,37 +1805,37 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" t="s">
         <v>101</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>102</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>103</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" t="s">
         <v>104</v>
       </c>
-      <c r="E11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>105</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>106</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>107</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>108</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>109</v>
-      </c>
-      <c r="K11" t="s">
-        <v>110</v>
       </c>
       <c r="L11" t="b">
         <v>1</v>
@@ -1846,37 +1843,37 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
         <v>111</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>112</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>113</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" t="s">
         <v>114</v>
       </c>
-      <c r="E12" t="s">
-        <v>114</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>115</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>116</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>117</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>118</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>119</v>
-      </c>
-      <c r="K12" t="s">
-        <v>120</v>
       </c>
       <c r="L12" t="b">
         <v>1</v>
@@ -1884,37 +1881,37 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" t="s">
         <v>121</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>122</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>123</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" t="s">
         <v>124</v>
       </c>
-      <c r="E13" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>125</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>126</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>127</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>128</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>129</v>
-      </c>
-      <c r="K13" t="s">
-        <v>130</v>
       </c>
       <c r="L13" t="b">
         <v>1</v>
@@ -1922,37 +1919,37 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B14" t="s">
         <v>131</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>132</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>133</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" t="s">
         <v>134</v>
       </c>
-      <c r="E14" t="s">
-        <v>134</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>135</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>136</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>137</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>138</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>139</v>
-      </c>
-      <c r="K14" t="s">
-        <v>140</v>
       </c>
       <c r="L14" t="b">
         <v>1</v>
@@ -1960,37 +1957,37 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" t="s">
         <v>141</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>142</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>143</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>143</v>
+      </c>
+      <c r="F15" t="s">
         <v>144</v>
       </c>
-      <c r="E15" t="s">
-        <v>144</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>145</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>146</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>147</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>148</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>149</v>
-      </c>
-      <c r="K15" t="s">
-        <v>150</v>
       </c>
       <c r="L15" t="b">
         <v>1</v>
@@ -1998,37 +1995,37 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" t="s">
         <v>151</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>152</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>153</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" t="s">
         <v>154</v>
       </c>
-      <c r="E16" t="s">
-        <v>154</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>155</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>156</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>157</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>158</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>159</v>
-      </c>
-      <c r="K16" t="s">
-        <v>160</v>
       </c>
       <c r="L16" t="b">
         <v>1</v>
@@ -2036,37 +2033,37 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" t="s">
         <v>161</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>162</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>163</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>163</v>
+      </c>
+      <c r="F17" t="s">
         <v>164</v>
       </c>
-      <c r="E17" t="s">
-        <v>164</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>165</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>166</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>167</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>168</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>169</v>
-      </c>
-      <c r="K17" t="s">
-        <v>170</v>
       </c>
       <c r="L17" t="b">
         <v>1</v>
@@ -2074,37 +2071,37 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" t="s">
         <v>171</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>172</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>173</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" t="s">
         <v>174</v>
       </c>
-      <c r="E18" t="s">
-        <v>174</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>175</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>176</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>177</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>178</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>179</v>
-      </c>
-      <c r="K18" t="s">
-        <v>180</v>
       </c>
       <c r="L18" t="b">
         <v>1</v>
@@ -2112,37 +2109,37 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>180</v>
+      </c>
+      <c r="B19" t="s">
         <v>181</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>182</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>183</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
+        <v>183</v>
+      </c>
+      <c r="F19" t="s">
         <v>184</v>
       </c>
-      <c r="E19" t="s">
-        <v>184</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>185</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>186</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>187</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>188</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>189</v>
-      </c>
-      <c r="K19" t="s">
-        <v>190</v>
       </c>
       <c r="L19" t="b">
         <v>1</v>
@@ -2150,28 +2147,28 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" t="s">
         <v>191</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>192</v>
-      </c>
-      <c r="C20" t="s">
-        <v>193</v>
       </c>
       <c r="D20">
         <v>1143</v>
       </c>
       <c r="E20" t="s">
+        <v>193</v>
+      </c>
+      <c r="I20" t="s">
         <v>194</v>
       </c>
-      <c r="I20" t="s">
-        <v>195</v>
-      </c>
       <c r="J20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="K20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L20" t="b">
         <v>1</v>
@@ -2179,37 +2176,37 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>197</v>
+      </c>
+      <c r="B21" t="s">
         <v>198</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>199</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>200</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>200</v>
+      </c>
+      <c r="F21" t="s">
         <v>201</v>
       </c>
-      <c r="E21" t="s">
-        <v>201</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>202</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>203</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>204</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>205</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>206</v>
-      </c>
-      <c r="K21" t="s">
-        <v>207</v>
       </c>
       <c r="L21" t="b">
         <v>1</v>
@@ -2217,37 +2214,37 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>207</v>
+      </c>
+      <c r="B22" t="s">
         <v>208</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>209</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>210</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
+        <v>210</v>
+      </c>
+      <c r="F22" t="s">
         <v>211</v>
       </c>
-      <c r="E22" t="s">
-        <v>211</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>212</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>213</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>214</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>215</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>216</v>
-      </c>
-      <c r="K22" t="s">
-        <v>217</v>
       </c>
       <c r="L22" t="b">
         <v>1</v>
@@ -2255,37 +2252,37 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>217</v>
+      </c>
+      <c r="B23" t="s">
         <v>218</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
+        <v>217</v>
+      </c>
+      <c r="D23" t="s">
         <v>219</v>
       </c>
-      <c r="C23" t="s">
-        <v>218</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>219</v>
+      </c>
+      <c r="F23" t="s">
         <v>220</v>
       </c>
-      <c r="E23" t="s">
-        <v>220</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>221</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>222</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>223</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>224</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>225</v>
-      </c>
-      <c r="K23" t="s">
-        <v>226</v>
       </c>
       <c r="L23" t="b">
         <v>1</v>
@@ -2293,37 +2290,37 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>226</v>
+      </c>
+      <c r="B24" t="s">
         <v>227</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>228</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>229</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>229</v>
+      </c>
+      <c r="F24" t="s">
         <v>230</v>
       </c>
-      <c r="E24" t="s">
-        <v>230</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>231</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>232</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>233</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>234</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>235</v>
-      </c>
-      <c r="K24" t="s">
-        <v>236</v>
       </c>
       <c r="L24" t="b">
         <v>1</v>
@@ -2331,37 +2328,37 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>236</v>
+      </c>
+      <c r="B25" t="s">
         <v>237</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>238</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>239</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>239</v>
+      </c>
+      <c r="F25" t="s">
         <v>240</v>
       </c>
-      <c r="E25" t="s">
-        <v>240</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>241</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>242</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>243</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>244</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>245</v>
-      </c>
-      <c r="K25" t="s">
-        <v>246</v>
       </c>
       <c r="L25" t="b">
         <v>1</v>
@@ -2369,31 +2366,31 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>246</v>
+      </c>
+      <c r="B26" t="s">
         <v>247</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>248</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>249</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
+        <v>249</v>
+      </c>
+      <c r="F26" t="s">
         <v>250</v>
       </c>
-      <c r="E26" t="s">
-        <v>250</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="I26" t="s">
+        <v>194</v>
+      </c>
+      <c r="J26" t="s">
+        <v>339</v>
+      </c>
+      <c r="K26" t="s">
         <v>251</v>
-      </c>
-      <c r="I26" t="s">
-        <v>195</v>
-      </c>
-      <c r="J26" t="s">
-        <v>340</v>
-      </c>
-      <c r="K26" t="s">
-        <v>252</v>
       </c>
       <c r="L26" t="b">
         <v>1</v>
@@ -2401,31 +2398,31 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>252</v>
+      </c>
+      <c r="B27" t="s">
         <v>253</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>252</v>
+      </c>
+      <c r="D27" t="s">
         <v>254</v>
       </c>
-      <c r="C27" t="s">
-        <v>253</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
+        <v>254</v>
+      </c>
+      <c r="F27" t="s">
+        <v>250</v>
+      </c>
+      <c r="I27" t="s">
+        <v>194</v>
+      </c>
+      <c r="J27" t="s">
+        <v>340</v>
+      </c>
+      <c r="K27" t="s">
         <v>255</v>
-      </c>
-      <c r="E27" t="s">
-        <v>255</v>
-      </c>
-      <c r="F27" t="s">
-        <v>251</v>
-      </c>
-      <c r="I27" t="s">
-        <v>195</v>
-      </c>
-      <c r="J27" t="s">
-        <v>341</v>
-      </c>
-      <c r="K27" t="s">
-        <v>256</v>
       </c>
       <c r="L27" t="b">
         <v>1</v>
@@ -2433,37 +2430,37 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>256</v>
+      </c>
+      <c r="B28" t="s">
         <v>257</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>258</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>259</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
+        <v>259</v>
+      </c>
+      <c r="F28" t="s">
         <v>260</v>
       </c>
-      <c r="E28" t="s">
-        <v>260</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>261</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>262</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>263</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>264</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>265</v>
-      </c>
-      <c r="K28" t="s">
-        <v>266</v>
       </c>
       <c r="L28" t="b">
         <v>1</v>
@@ -2471,37 +2468,37 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>266</v>
+      </c>
+      <c r="B29" t="s">
         <v>267</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>268</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>269</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
+        <v>269</v>
+      </c>
+      <c r="F29" t="s">
         <v>270</v>
       </c>
-      <c r="E29" t="s">
-        <v>270</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>271</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>272</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>273</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>274</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>275</v>
-      </c>
-      <c r="K29" t="s">
-        <v>276</v>
       </c>
       <c r="L29" t="b">
         <v>1</v>
@@ -2509,37 +2506,37 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>276</v>
+      </c>
+      <c r="B30" t="s">
         <v>277</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>278</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>279</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
+        <v>279</v>
+      </c>
+      <c r="F30" t="s">
         <v>280</v>
       </c>
-      <c r="E30" t="s">
-        <v>280</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>281</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>282</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>283</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>284</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>285</v>
-      </c>
-      <c r="K30" t="s">
-        <v>286</v>
       </c>
       <c r="L30" t="b">
         <v>1</v>
@@ -2547,37 +2544,37 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>286</v>
+      </c>
+      <c r="B31" t="s">
         <v>287</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>288</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>289</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
+        <v>289</v>
+      </c>
+      <c r="F31" t="s">
         <v>290</v>
       </c>
-      <c r="E31" t="s">
-        <v>290</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>291</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>292</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>293</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
+        <v>341</v>
+      </c>
+      <c r="K31" t="s">
         <v>294</v>
-      </c>
-      <c r="J31" t="s">
-        <v>342</v>
-      </c>
-      <c r="K31" t="s">
-        <v>295</v>
       </c>
       <c r="L31" t="b">
         <v>1</v>
@@ -2585,37 +2582,37 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>295</v>
+      </c>
+      <c r="B32" t="s">
         <v>296</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>297</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>298</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
+        <v>298</v>
+      </c>
+      <c r="F32" t="s">
         <v>299</v>
       </c>
-      <c r="E32" t="s">
-        <v>299</v>
-      </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>300</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>301</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>302</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>303</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>304</v>
-      </c>
-      <c r="K32" t="s">
-        <v>305</v>
       </c>
       <c r="L32" t="b">
         <v>1</v>
@@ -2623,37 +2620,37 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>305</v>
+      </c>
+      <c r="B33" t="s">
         <v>306</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>307</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>308</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
+        <v>308</v>
+      </c>
+      <c r="F33" t="s">
         <v>309</v>
       </c>
-      <c r="E33" t="s">
-        <v>309</v>
-      </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>310</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>311</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>312</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>313</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>314</v>
-      </c>
-      <c r="K33" t="s">
-        <v>315</v>
       </c>
       <c r="L33" t="b">
         <v>1</v>
@@ -2661,37 +2658,37 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>315</v>
+      </c>
+      <c r="B34" t="s">
         <v>316</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>317</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>318</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
+        <v>318</v>
+      </c>
+      <c r="F34" t="s">
         <v>319</v>
       </c>
-      <c r="E34" t="s">
-        <v>319</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>320</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>321</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>322</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>323</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>324</v>
-      </c>
-      <c r="K34" t="s">
-        <v>325</v>
       </c>
       <c r="L34" t="b">
         <v>1</v>
@@ -2699,22 +2696,22 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>325</v>
+      </c>
+      <c r="B35" t="s">
         <v>326</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
+        <v>325</v>
+      </c>
+      <c r="I35" t="s">
+        <v>194</v>
+      </c>
+      <c r="J35" t="s">
+        <v>195</v>
+      </c>
+      <c r="K35" t="s">
         <v>327</v>
-      </c>
-      <c r="C35" t="s">
-        <v>326</v>
-      </c>
-      <c r="I35" t="s">
-        <v>195</v>
-      </c>
-      <c r="J35" t="s">
-        <v>196</v>
-      </c>
-      <c r="K35" t="s">
-        <v>328</v>
       </c>
       <c r="L35" t="b">
         <v>0</v>
@@ -2722,37 +2719,37 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>328</v>
+      </c>
+      <c r="B36" t="s">
         <v>329</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>330</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>331</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
+        <v>331</v>
+      </c>
+      <c r="F36" t="s">
         <v>332</v>
       </c>
-      <c r="E36" t="s">
-        <v>332</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>333</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>334</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>335</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>336</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>337</v>
-      </c>
-      <c r="K36" t="s">
-        <v>338</v>
       </c>
       <c r="L36" t="b">
         <v>1</v>

</xml_diff>